<commit_message>
reworked dur calc, lots of other changes
</commit_message>
<xml_diff>
--- a/Prelim_Data/Central_Valley/Central_Valley_30_95.xlsx
+++ b/Prelim_Data/Central_Valley/Central_Valley_30_95.xlsx
@@ -794,7 +794,7 @@
         <v>18.99019607843137</v>
       </c>
       <c r="O3" t="n">
-        <v>0.00663858965714238</v>
+        <v>0.006638589657142382</v>
       </c>
       <c r="P3" t="n">
         <v>0.5666666666666667</v>
@@ -915,7 +915,7 @@
         <v>7.574561403508771</v>
       </c>
       <c r="O4" t="n">
-        <v>0.01689687697811003</v>
+        <v>0.01689687697811004</v>
       </c>
       <c r="P4" t="n">
         <v>0.6333333333333333</v>
@@ -1762,7 +1762,7 @@
         <v>7.2612012987013</v>
       </c>
       <c r="O11" t="n">
-        <v>0.3414642721151772</v>
+        <v>0.3414642721151773</v>
       </c>
       <c r="P11" t="n">
         <v>0.7333333333333333</v>
@@ -2004,7 +2004,7 @@
         <v>2.483722342472342</v>
       </c>
       <c r="O13" t="n">
-        <v>0.004462361544591269</v>
+        <v>0.00446236154459127</v>
       </c>
       <c r="P13" t="n">
         <v>1</v>
@@ -2076,7 +2076,7 @@
         </is>
       </c>
       <c r="AK13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -2125,7 +2125,7 @@
         <v>3.327207019171305</v>
       </c>
       <c r="O14" t="n">
-        <v>0.008533913737589294</v>
+        <v>0.008533913737589298</v>
       </c>
       <c r="P14" t="n">
         <v>0.9333333333333333</v>
@@ -2197,7 +2197,7 @@
         </is>
       </c>
       <c r="AK14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -2851,7 +2851,7 @@
         <v>2.504842472342472</v>
       </c>
       <c r="O20" t="n">
-        <v>0.003961376155322858</v>
+        <v>0.00396137615532286</v>
       </c>
       <c r="P20" t="n">
         <v>1</v>
@@ -2972,7 +2972,7 @@
         <v>4.882673675530818</v>
       </c>
       <c r="O21" t="n">
-        <v>0.09449115251611293</v>
+        <v>0.09449115251611298</v>
       </c>
       <c r="P21" t="n">
         <v>0.7</v>
@@ -4545,7 +4545,7 @@
         <v>14.67361111111111</v>
       </c>
       <c r="O34" t="n">
-        <v>0.01688877555810497</v>
+        <v>0.01688877555810498</v>
       </c>
       <c r="P34" t="n">
         <v>0.4</v>
@@ -4787,7 +4787,7 @@
         <v>5.653968253968254</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0009109086966998172</v>
+        <v>0.0009109086966998175</v>
       </c>
       <c r="P36" t="n">
         <v>0.7</v>
@@ -4859,7 +4859,7 @@
         </is>
       </c>
       <c r="AK36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -4980,7 +4980,7 @@
         </is>
       </c>
       <c r="AK37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -5150,7 +5150,7 @@
         <v>31.4</v>
       </c>
       <c r="O39" t="n">
-        <v>0.3538675491995118</v>
+        <v>0.353867549199511</v>
       </c>
       <c r="P39" t="n">
         <v>0.2631578947368421</v>
@@ -5343,7 +5343,7 @@
         </is>
       </c>
       <c r="AK40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -5464,7 +5464,7 @@
         </is>
       </c>
       <c r="AK41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -5513,7 +5513,7 @@
         <v>36.88888888888889</v>
       </c>
       <c r="O42" t="n">
-        <v>0.5536757223203921</v>
+        <v>0.5536757223203924</v>
       </c>
       <c r="P42" t="n">
         <v>0.3</v>
@@ -5634,7 +5634,7 @@
         <v>6.229714285714286</v>
       </c>
       <c r="O43" t="n">
-        <v>0.003720445005879517</v>
+        <v>0.003720445005879518</v>
       </c>
       <c r="P43" t="n">
         <v>0.8333333333333334</v>
@@ -5706,7 +5706,7 @@
         </is>
       </c>
       <c r="AK43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -5827,7 +5827,7 @@
         </is>
       </c>
       <c r="AK44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -6723,7 +6723,7 @@
         <v>3.189420995670996</v>
       </c>
       <c r="O52" t="n">
-        <v>0.0007259547207608326</v>
+        <v>0.0007259547207608328</v>
       </c>
       <c r="P52" t="n">
         <v>0.9333333333333333</v>
@@ -6795,7 +6795,7 @@
         </is>
       </c>
       <c r="AK52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -7086,7 +7086,7 @@
         <v>13.85454545454546</v>
       </c>
       <c r="O55" t="n">
-        <v>0.06873677721530221</v>
+        <v>0.06873677721530226</v>
       </c>
       <c r="P55" t="n">
         <v>0.3666666666666666</v>
@@ -7207,7 +7207,7 @@
         <v>16.44090909090909</v>
       </c>
       <c r="O56" t="n">
-        <v>0.0887961370574783</v>
+        <v>0.08879613705747835</v>
       </c>
       <c r="P56" t="n">
         <v>0.3666666666666666</v>
@@ -7449,7 +7449,7 @@
         <v>34.27291666666667</v>
       </c>
       <c r="O58" t="n">
-        <v>0.7306720040936669</v>
+        <v>0.7306720040936679</v>
       </c>
       <c r="P58" t="n">
         <v>0.2666666666666667</v>
@@ -7763,7 +7763,7 @@
         </is>
       </c>
       <c r="AK60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -7933,7 +7933,7 @@
         <v>4.325396825396824</v>
       </c>
       <c r="O62" t="n">
-        <v>0.0009916035592921024</v>
+        <v>0.0009916035592921026</v>
       </c>
       <c r="P62" t="n">
         <v>0.9</v>
@@ -8538,7 +8538,7 @@
         <v>19.84375</v>
       </c>
       <c r="O67" t="n">
-        <v>0.01099562600072402</v>
+        <v>0.01099562600072403</v>
       </c>
       <c r="P67" t="n">
         <v>0.4444444444444444</v>
@@ -8852,7 +8852,7 @@
         </is>
       </c>
       <c r="AK69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -9143,7 +9143,7 @@
         <v>3.296323312702623</v>
       </c>
       <c r="O72" t="n">
-        <v>0.007682911412505885</v>
+        <v>0.007682911412505886</v>
       </c>
       <c r="P72" t="n">
         <v>0.9666666666666667</v>
@@ -9336,7 +9336,7 @@
         </is>
       </c>
       <c r="AK73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -9627,7 +9627,7 @@
         <v>2.225411413205531</v>
       </c>
       <c r="O76" t="n">
-        <v>0.0009276591751838548</v>
+        <v>0.0009276591751838549</v>
       </c>
       <c r="P76" t="n">
         <v>1</v>
@@ -9990,7 +9990,7 @@
         <v>3.970197044334975</v>
       </c>
       <c r="O79" t="n">
-        <v>0.01676367222418532</v>
+        <v>0.01676367222418533</v>
       </c>
       <c r="P79" t="n">
         <v>0.9666666666666667</v>
@@ -16157,32 +16157,32 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>increasing</t>
+          <t>no trend</t>
         </is>
       </c>
       <c r="L5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0356289338830702</v>
+        <v>0.1544237061170961</v>
       </c>
       <c r="N5" t="n">
-        <v>2.101137089783457</v>
+        <v>1.424078649513432</v>
       </c>
       <c r="O5" t="n">
-        <v>0.1770114942528736</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="P5" t="n">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="Q5" t="n">
-        <v>1308.333333333333</v>
+        <v>83.33333333333333</v>
       </c>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>-2.666666666666667</v>
       </c>
     </row>
     <row r="6">
@@ -17854,19 +17854,19 @@
         <v>0</v>
       </c>
       <c r="M31" t="n">
-        <v>0.8519235454668399</v>
+        <v>0.9311749148236654</v>
       </c>
       <c r="N31" t="n">
-        <v>-0.186664686512228</v>
+        <v>-0.08636670341750609</v>
       </c>
       <c r="O31" t="n">
-        <v>-0.02298850574712644</v>
+        <v>-0.01231527093596059</v>
       </c>
       <c r="P31" t="n">
-        <v>-10</v>
+        <v>-5</v>
       </c>
       <c r="Q31" t="n">
-        <v>2324.666666666667</v>
+        <v>2145</v>
       </c>
       <c r="R31" t="n">
         <v>0</v>
@@ -19797,32 +19797,32 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>increasing</t>
+          <t>no trend</t>
         </is>
       </c>
       <c r="L61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M61" t="n">
-        <v>0.0250783871751048</v>
+        <v>0.213590891281481</v>
       </c>
       <c r="N61" t="n">
-        <v>2.240193134720572</v>
+        <v>1.243751891458663</v>
       </c>
       <c r="O61" t="n">
-        <v>0.2850574712643678</v>
+        <v>0.1897233201581028</v>
       </c>
       <c r="P61" t="n">
-        <v>124</v>
+        <v>48</v>
       </c>
       <c r="Q61" t="n">
-        <v>3014.666666666667</v>
+        <v>1428</v>
       </c>
       <c r="R61" t="n">
-        <v>0.08461538461538462</v>
+        <v>0.08333333333333337</v>
       </c>
       <c r="S61" t="n">
-        <v>1.035576923076923</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="62">
@@ -20909,25 +20909,25 @@
         <v>0</v>
       </c>
       <c r="M78" t="n">
-        <v>0.6027403689644599</v>
+        <v>0.5807172923623485</v>
       </c>
       <c r="N78" t="n">
-        <v>0.5204637762700459</v>
+        <v>-0.5523372814706976</v>
       </c>
       <c r="O78" t="n">
-        <v>0.06896551724137931</v>
+        <v>-0.08</v>
       </c>
       <c r="P78" t="n">
-        <v>30</v>
+        <v>-26</v>
       </c>
       <c r="Q78" t="n">
-        <v>3104.666666666667</v>
+        <v>2048.666666666667</v>
       </c>
       <c r="R78" t="n">
-        <v>0.01282051282051281</v>
+        <v>-0.02083333333333333</v>
       </c>
       <c r="S78" t="n">
-        <v>2.814102564102564</v>
+        <v>3.59375</v>
       </c>
     </row>
     <row r="79">
@@ -21162,32 +21162,32 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>increasing</t>
+          <t>no trend</t>
         </is>
       </c>
       <c r="L82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M82" t="n">
-        <v>0.03413533845483663</v>
+        <v>0.3513050661832442</v>
       </c>
       <c r="N82" t="n">
-        <v>2.118469344749569</v>
+        <v>-0.9320608751309648</v>
       </c>
       <c r="O82" t="n">
-        <v>0.2528735632183908</v>
+        <v>-0.1978021978021978</v>
       </c>
       <c r="P82" t="n">
-        <v>110</v>
+        <v>-18</v>
       </c>
       <c r="Q82" t="n">
-        <v>2647.333333333333</v>
+        <v>332.6666666666667</v>
       </c>
       <c r="R82" t="n">
-        <v>0</v>
+        <v>-0.11875</v>
       </c>
       <c r="S82" t="n">
-        <v>0</v>
+        <v>3.549652777777778</v>
       </c>
     </row>
   </sheetData>
@@ -21545,25 +21545,25 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.05634718979713216</v>
+        <v>0.5084542305885602</v>
       </c>
       <c r="N5" t="n">
-        <v>1.90834074680476</v>
+        <v>0.6612465225335806</v>
       </c>
       <c r="O5" t="n">
-        <v>0.1609195402298851</v>
+        <v>0.1944444444444444</v>
       </c>
       <c r="P5" t="n">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="Q5" t="n">
-        <v>1307.333333333333</v>
+        <v>82.33333333333333</v>
       </c>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>0.6666666666666667</v>
       </c>
     </row>
     <row r="6">
@@ -23235,19 +23235,19 @@
         <v>0</v>
       </c>
       <c r="M31" t="n">
-        <v>1</v>
+        <v>0.9308309497786535</v>
       </c>
       <c r="N31" t="n">
-        <v>0</v>
+        <v>0.08679941859050837</v>
       </c>
       <c r="O31" t="n">
-        <v>0</v>
+        <v>0.01231527093596059</v>
       </c>
       <c r="P31" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q31" t="n">
-        <v>2303.333333333333</v>
+        <v>2123.666666666667</v>
       </c>
       <c r="R31" t="n">
         <v>0</v>
@@ -25185,25 +25185,25 @@
         <v>0</v>
       </c>
       <c r="M61" t="n">
-        <v>0.3319298995301962</v>
+        <v>0.5742632659400388</v>
       </c>
       <c r="N61" t="n">
-        <v>0.9702339343681315</v>
+        <v>-0.5617838953175571</v>
       </c>
       <c r="O61" t="n">
-        <v>0.1241379310344828</v>
+        <v>-0.08695652173913043</v>
       </c>
       <c r="P61" t="n">
-        <v>54</v>
+        <v>-22</v>
       </c>
       <c r="Q61" t="n">
-        <v>2984</v>
+        <v>1397.333333333333</v>
       </c>
       <c r="R61" t="n">
         <v>0</v>
       </c>
       <c r="S61" t="n">
-        <v>3.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
@@ -26290,25 +26290,25 @@
         <v>0</v>
       </c>
       <c r="M78" t="n">
-        <v>0.3122426509065117</v>
+        <v>1</v>
       </c>
       <c r="N78" t="n">
-        <v>1.010527458339114</v>
+        <v>0</v>
       </c>
       <c r="O78" t="n">
-        <v>0.1310344827586207</v>
+        <v>0.003076923076923077</v>
       </c>
       <c r="P78" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="Q78" t="n">
-        <v>3071</v>
+        <v>2015</v>
       </c>
       <c r="R78" t="n">
-        <v>0.0625</v>
+        <v>0</v>
       </c>
       <c r="S78" t="n">
-        <v>2.59375</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79">
@@ -26543,32 +26543,32 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>increasing</t>
+          <t>no trend</t>
         </is>
       </c>
       <c r="L82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M82" t="n">
-        <v>0.01069571328331698</v>
+        <v>0.866677633709956</v>
       </c>
       <c r="N82" t="n">
-        <v>2.552486244596326</v>
+        <v>0.1678800645554932</v>
       </c>
       <c r="O82" t="n">
-        <v>0.303448275862069</v>
+        <v>0.04395604395604396</v>
       </c>
       <c r="P82" t="n">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="Q82" t="n">
-        <v>2634</v>
+        <v>319.3333333333333</v>
       </c>
       <c r="R82" t="n">
-        <v>0.03448275862068965</v>
+        <v>0</v>
       </c>
       <c r="S82" t="n">
-        <v>-0.5</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>